<commit_message>
update map and sample
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -415,12 +415,12 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>S_i</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>pi_ij</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>S_i</t>
         </is>
       </c>
     </row>
@@ -463,10 +463,10 @@
         <v>5.033221123989189</v>
       </c>
       <c r="L2">
+        <v>1.34500506230837</v>
+      </c>
+      <c r="M2">
         <v>0.3560491898015857</v>
-      </c>
-      <c r="M2">
-        <v>1.34500506230837</v>
       </c>
     </row>
     <row r="3">
@@ -508,10 +508,10 @@
         <v>7.811709119669064</v>
       </c>
       <c r="L3">
+        <v>2.195833495081968</v>
+      </c>
+      <c r="M3">
         <v>0.6907608859996458</v>
-      </c>
-      <c r="M3">
-        <v>2.195833495081968</v>
       </c>
     </row>
     <row r="4">
@@ -553,10 +553,10 @@
         <v>7.867004136244687</v>
       </c>
       <c r="L4">
+        <v>2.923035284378024</v>
+      </c>
+      <c r="M4">
         <v>0.3795520420812715</v>
-      </c>
-      <c r="M4">
-        <v>2.923035284378024</v>
       </c>
     </row>
     <row r="5">
@@ -598,10 +598,10 @@
         <v>10.92066372540615</v>
       </c>
       <c r="L5">
+        <v>3.666704720512436</v>
+      </c>
+      <c r="M5">
         <v>0.4929591716088889</v>
-      </c>
-      <c r="M5">
-        <v>3.666704720512436</v>
       </c>
     </row>
     <row r="6">
@@ -643,10 +643,10 @@
         <v>10.32150990243152</v>
       </c>
       <c r="L6">
+        <v>1.869498397456427</v>
+      </c>
+      <c r="M6">
         <v>0.6771661247679462</v>
-      </c>
-      <c r="M6">
-        <v>1.869498397456427</v>
       </c>
     </row>
     <row r="7">
@@ -688,10 +688,10 @@
         <v>10.4154691496963</v>
       </c>
       <c r="L7">
+        <v>1.596580571274171</v>
+      </c>
+      <c r="M7">
         <v>0.5080785761963192</v>
-      </c>
-      <c r="M7">
-        <v>1.596580571274171</v>
       </c>
     </row>
     <row r="8">
@@ -733,10 +733,10 @@
         <v>11.32294307076384</v>
       </c>
       <c r="L8">
+        <v>2.431184583093056</v>
+      </c>
+      <c r="M8">
         <v>0.1917089569249553</v>
-      </c>
-      <c r="M8">
-        <v>2.431184583093056</v>
       </c>
     </row>
     <row r="9">
@@ -778,10 +778,10 @@
         <v>4.322101247490338</v>
       </c>
       <c r="L9">
+        <v>1.851542443097899</v>
+      </c>
+      <c r="M9">
         <v>0.2092529809640788</v>
-      </c>
-      <c r="M9">
-        <v>1.851542443097899</v>
       </c>
     </row>
     <row r="10">
@@ -823,10 +823,10 @@
         <v>10.00628015682746</v>
       </c>
       <c r="L10">
+        <v>2.550556141662226</v>
+      </c>
+      <c r="M10">
         <v>0.4264872700548309</v>
-      </c>
-      <c r="M10">
-        <v>2.550556141662226</v>
       </c>
     </row>
     <row r="11">
@@ -868,10 +868,10 @@
         <v>14.71894798188444</v>
       </c>
       <c r="L11">
+        <v>2.750600649797019</v>
+      </c>
+      <c r="M11">
         <v>0.1917668086695493</v>
-      </c>
-      <c r="M11">
-        <v>2.750600649797019</v>
       </c>
     </row>
     <row r="12">
@@ -913,10 +913,10 @@
         <v>9.558632809590966</v>
       </c>
       <c r="L12">
+        <v>2.770239526489727</v>
+      </c>
+      <c r="M12">
         <v>0.3209874353744993</v>
-      </c>
-      <c r="M12">
-        <v>2.770239526489727</v>
       </c>
     </row>
     <row r="13">
@@ -958,10 +958,10 @@
         <v>7.880812539818971</v>
       </c>
       <c r="L13">
+        <v>1.600357775092295</v>
+      </c>
+      <c r="M13">
         <v>0.4043563822702481</v>
-      </c>
-      <c r="M13">
-        <v>1.600357775092295</v>
       </c>
     </row>
     <row r="14">
@@ -1003,10 +1003,10 @@
         <v>5.475207039068142</v>
       </c>
       <c r="L14">
+        <v>1.350764558945041</v>
+      </c>
+      <c r="M14">
         <v>0.418539020319033</v>
-      </c>
-      <c r="M14">
-        <v>1.350764558945041</v>
       </c>
     </row>
     <row r="15">
@@ -1048,10 +1048,10 @@
         <v>2.43724515948041</v>
       </c>
       <c r="L15">
+        <v>2.025986572473288</v>
+      </c>
+      <c r="M15">
         <v>0.3853734671627302</v>
-      </c>
-      <c r="M15">
-        <v>2.025986572473288</v>
       </c>
     </row>
     <row r="16">
@@ -1093,10 +1093,10 @@
         <v>4.989452412647309</v>
       </c>
       <c r="L16">
+        <v>3.017487262468767</v>
+      </c>
+      <c r="M16">
         <v>0.1769486667957952</v>
-      </c>
-      <c r="M16">
-        <v>3.017487262468767</v>
       </c>
     </row>
   </sheetData>

</xml_diff>